<commit_message>
initial commit, imported packages, imported excel data
</commit_message>
<xml_diff>
--- a/data/proshares_analysis_data.xlsx
+++ b/data/proshares_analysis_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markhendricks/Projects/finm-portfolio-2023/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b99f5ce6d853cb8b/Desktop/UChicago/FINM_36700/finm-portfolio-2023-2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3E2837-6EFD-044F-9143-34C913804368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4C3E2837-6EFD-044F-9143-34C913804368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BA6178B-0725-4B87-A75D-300B67A9EC93}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-1460" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="13680" windowHeight="12105" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="descriptions" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -188,7 +188,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -498,16 +498,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -515,7 +515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -523,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -531,7 +531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -547,7 +547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -555,7 +555,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -563,7 +563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -579,7 +579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -587,7 +587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -595,7 +595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -603,7 +603,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -611,7 +611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -619,7 +619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -638,9 +638,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
@@ -657,7 +660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>40786</v>
       </c>
@@ -677,7 +680,7 @@
         <v>-6.4908521101463279E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>40816</v>
       </c>
@@ -697,7 +700,7 @@
         <v>-2.2143257901626971E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>40847</v>
       </c>
@@ -717,7 +720,7 @@
         <v>2.5241513555785081E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>40877</v>
       </c>
@@ -737,7 +740,7 @@
         <v>-7.9634865230115981E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>40908</v>
       </c>
@@ -757,7 +760,7 @@
         <v>1.8177639414136419E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>40939</v>
       </c>
@@ -777,7 +780,7 @@
         <v>1.698923834153665E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>40968</v>
       </c>
@@ -797,7 +800,7 @@
         <v>1.3071493316599179E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>40999</v>
       </c>
@@ -817,7 +820,7 @@
         <v>-6.0931174089069451E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>41029</v>
       </c>
@@ -837,7 +840,7 @@
         <v>-2.8839691236073328E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>41060</v>
       </c>
@@ -857,7 +860,7 @@
         <v>-1.2659986028669801E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>41090</v>
       </c>
@@ -877,7 +880,7 @@
         <v>7.3276290093011731E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>41121</v>
       </c>
@@ -897,7 +900,7 @@
         <v>1.23634780394235E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>41152</v>
       </c>
@@ -917,7 +920,7 @@
         <v>6.8243876511855373E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>41182</v>
       </c>
@@ -937,7 +940,7 @@
         <v>4.6383049030629397E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>41213</v>
       </c>
@@ -957,7 +960,7 @@
         <v>1.419964540998464E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>41243</v>
       </c>
@@ -977,7 +980,7 @@
         <v>1.7704361201011929E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>41274</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>-4.6101928044205431E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>41305</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>5.6518508104199672E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>41333</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>-2.5564005879719082E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>41364</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>7.47538835261774E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>41394</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>9.6169480367545024E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>41425</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>7.0310781510207754E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>41455</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>-2.7755207781349659E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>41486</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>1.987549052855964E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>41517</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>-1.0276507729153121E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>41547</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>2.291425851635287E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>41578</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>1.4701972253937431E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>41608</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>6.5547112227752891E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>41639</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>5.3864912771000029E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>41670</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>-7.592835166174261E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>41698</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>2.086930497041695E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>41729</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>-4.4313146233383449E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>41759</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>2.397293889354613E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>41790</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>1.4338064982656549E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>41820</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>9.4235938869167146E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>41851</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>-1.300292059942176E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>41882</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>1.89172166796483E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>41912</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>-1.6243420884189289E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>41943</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>3.706843345900213E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>41973</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>1.20870206216499E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>42004</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>-1.18767888383805E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>42035</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>-1.327150090563267E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>42063</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>3.4141159335420612E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>42094</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>-1.6697581391634799E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>42124</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>2.0034250933538278E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>42155</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>-3.302126424268303E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>42185</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>-1.3673867196149381E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>42216</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>-3.3490111216616381E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>42247</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>-1.69089684167123E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>42277</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>-9.2908125435331446E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>42308</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>8.6824389451045647E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>42338</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>-5.1638723796533226E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>42369</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>-1.046798957344541E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>42400</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>-1.4054214551365241E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>42429</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>3.563637767610484E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>42460</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>2.3437259548798162E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>42490</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>8.326441620930769E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>42521</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>-3.4410125449698681E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>42551</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>6.9057879930567454E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>42582</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>7.8875604663430909E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>42613</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>-2.7204264213122049E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>42643</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>-3.4375311872791858E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>42674</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>-1.365132187095597E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>42704</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>-1.349537783309218E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>42735</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>5.6315977473608836E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>42766</v>
       </c>
@@ -1977,7 +1980,7 @@
         <v>2.0934099153568919E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>42794</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>1.2575699299380849E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>42825</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>-4.4687910802920783E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>42855</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>2.405806708700053E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>42886</v>
       </c>
@@ -2057,7 +2060,7 @@
         <v>4.4582650661495471E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>42916</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>4.0981939096695896E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>42947</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>9.1796177123892875E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>42978</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>5.0517770647862106E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>43008</v>
       </c>
@@ -2137,7 +2140,7 @@
         <v>1.677882816954579E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>43039</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>8.3681098151255906E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>43069</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>5.9723066191565977E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>43100</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>4.2891149411319329E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>43131</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>2.0040714931418121E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>43159</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>-1.352713976183584E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>43190</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>-4.8986319199807449E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>43220</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>-2.623095323568303E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>43251</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>6.5785487992189307E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>43281</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>-6.8612699368040264E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>43312</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>8.883597072548044E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>43343</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>2.6076909214902688E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>43373</v>
       </c>
@@ -2377,7 +2380,7 @@
         <v>-6.4846500579740507E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>43404</v>
       </c>
@@ -2397,7 +2400,7 @@
         <v>-2.7672862820607769E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>43434</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>2.680294215787304E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>43465</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>-1.738800166392351E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>43496</v>
       </c>
@@ -2457,7 +2460,7 @@
         <v>2.7701289904582541E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>43524</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>8.7580102660356207E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>43555</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>4.3427621813947326E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>43585</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>6.6503795418628719E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>43616</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>-1.304781506170938E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>43646</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>1.8241538467013148E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>43677</v>
       </c>
@@ -2577,7 +2580,7 @@
         <v>-1.3140742242243599E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>43708</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>-2.9640568734974342E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>43738</v>
       </c>
@@ -2617,7 +2620,7 @@
         <v>4.292583622898416E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>43769</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>9.5340278821387514E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>43799</v>
       </c>
@@ -2657,7 +2660,7 @@
         <v>4.8847023308788984E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>43830</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>1.707019622974304E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>43861</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>-5.8463487418155546E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>43890</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>-1.469500955703729E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>43921</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>-5.6347427970731889E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>43951</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>3.0909550629733881E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>43982</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>1.9763407837115391E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>44012</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>1.302947491704076E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>44043</v>
       </c>
@@ -2817,7 +2820,7 @@
         <v>1.7809831191978761E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>44074</v>
       </c>
@@ -2837,7 +2840,7 @@
         <v>1.2636831393972869E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>44104</v>
       </c>
@@ -2857,7 +2860,7 @@
         <v>-8.3194231154437581E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>44135</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>-4.5177883709029984E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>44165</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>3.3387892027892718E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>44196</v>
       </c>
@@ -2917,7 +2920,7 @@
         <v>2.1496896056338869E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>44227</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>1.2526109409638499E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>44255</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>1.8749660042425289E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>44286</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>-7.1792415169660284E-3</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>44316</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>5.9734235726669471E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>44347</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>5.9411512659319774E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="2">
         <v>44377</v>
       </c>
@@ -3037,7 +3040,7 @@
         <v>2.4857593327229921E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="2">
         <v>44408</v>
       </c>
@@ -3057,7 +3060,7 @@
         <v>-3.40865131558088E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="2">
         <v>44439</v>
       </c>
@@ -3077,7 +3080,7 @@
         <v>1.2440383201983709E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="2">
         <v>44469</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>-1.335917887444793E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="2">
         <v>44500</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>1.070579671869254E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" s="2">
         <v>44530</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>-1.495490902138241E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" s="2">
         <v>44561</v>
       </c>
@@ -3157,7 +3160,7 @@
         <v>8.1781331987564876E-3</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" s="2">
         <v>44592</v>
       </c>
@@ -3177,7 +3180,7 @@
         <v>-2.0760801553049161E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" s="2">
         <v>44620</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>-6.8124846399606476E-3</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" s="2">
         <v>44651</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>-2.5206535223163411E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" s="2">
         <v>44681</v>
       </c>
@@ -3237,7 +3240,7 @@
         <v>-3.3397060185491378E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" s="2">
         <v>44712</v>
       </c>
@@ -3257,7 +3260,7 @@
         <v>-4.0275805430561862E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" s="2">
         <v>44742</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>-3.368057225707588E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" s="2">
         <v>44773</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>1.882277648397368E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" s="2">
         <v>44804</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>-1.1631518518647851E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" s="2">
         <v>44834</v>
       </c>
@@ -3337,7 +3340,7 @@
         <v>-3.9807073046720598E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" s="2">
         <v>44865</v>
       </c>
@@ -3357,7 +3360,7 @@
         <v>1.477888667436433E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" s="2">
         <v>44895</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>3.9788230945676961E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" s="2">
         <v>44926</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>-8.1584716021759762E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" s="2">
         <v>44957</v>
       </c>
@@ -3417,7 +3420,7 @@
         <v>2.9163738580463731E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" s="2">
         <v>44985</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>-8.5353362922498954E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" s="2">
         <v>45016</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>5.853994490358172E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" s="2">
         <v>45046</v>
       </c>
@@ -3477,7 +3480,7 @@
         <v>5.135227661759556E-3</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" s="2">
         <v>45077</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>-6.4713896457765374E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" s="2">
         <v>45107</v>
       </c>
@@ -3517,7 +3520,7 @@
         <v>2.2625985601645301E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" s="2">
         <v>45138</v>
       </c>
@@ -3537,7 +3540,7 @@
         <v>1.9440160911833759E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" s="2">
         <v>45169</v>
       </c>
@@ -3568,9 +3571,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
@@ -3590,7 +3596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>40786</v>
       </c>
@@ -3613,7 +3619,7 @@
         <v>-8.8914708102029172E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>40816</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>-0.1115036366821149</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>40847</v>
       </c>
@@ -3659,7 +3665,7 @@
         <v>0.15100986465123661</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>40877</v>
       </c>
@@ -3682,7 +3688,7 @@
         <v>-3.7825793253146718E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>40908</v>
       </c>
@@ -3705,7 +3711,7 @@
         <v>5.1434659022435714E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>40939</v>
       </c>
@@ -3728,7 +3734,7 @@
         <v>7.1457803128157193E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>40968</v>
       </c>
@@ -3751,7 +3757,7 @@
         <v>2.5689152010312629E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>40999</v>
       </c>
@@ -3774,7 +3780,7 @@
         <v>2.4850828118499591E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>41029</v>
       </c>
@@ -3797,7 +3803,7 @@
         <v>-1.618063263434899E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>41060</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>-6.5791334004668522E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>41090</v>
       </c>
@@ -3843,7 +3849,7 @@
         <v>5.0523285712300137E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>41121</v>
       </c>
@@ -3866,7 +3872,7 @@
         <v>-1.5208913075754889E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>41152</v>
       </c>
@@ -3889,7 +3895,7 @@
         <v>3.535384445442924E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>41182</v>
       </c>
@@ -3912,7 +3918,7 @@
         <v>3.2605389008314667E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>41213</v>
       </c>
@@ -3935,7 +3941,7 @@
         <v>-2.169190128062648E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>41243</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>5.5118200138153384E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>41274</v>
       </c>
@@ -3981,7 +3987,7 @@
         <v>3.6157027725970632E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>41305</v>
       </c>
@@ -4004,7 +4010,7 @@
         <v>6.2408563146907348E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>41333</v>
       </c>
@@ -4027,7 +4033,7 @@
         <v>1.004679133180564E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>41364</v>
       </c>
@@ -4050,7 +4056,7 @@
         <v>4.6590150415580123E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>41394</v>
       </c>
@@ -4073,7 +4079,7 @@
         <v>-3.494499060815337E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>41425</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>3.9319702078960177E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>41455</v>
       </c>
@@ -4119,7 +4125,7 @@
         <v>-8.1790655962239445E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>41486</v>
       </c>
@@ -4142,7 +4148,7 @@
         <v>7.3290080197204066E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>41517</v>
       </c>
@@ -4165,7 +4171,7 @@
         <v>-3.1594307758516793E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>41547</v>
       </c>
@@ -4188,7 +4194,7 @@
         <v>6.4893715463380408E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>41578</v>
       </c>
@@ -4211,7 +4217,7 @@
         <v>2.4201222344640391E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>41608</v>
       </c>
@@ -4234,7 +4240,7 @@
         <v>3.9563130694185038E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>41639</v>
       </c>
@@ -4257,7 +4263,7 @@
         <v>2.020911400108627E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>41670</v>
       </c>
@@ -4280,7 +4286,7 @@
         <v>-2.7739425004691291E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>41698</v>
       </c>
@@ -4303,7 +4309,7 @@
         <v>4.7788444836318611E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>41729</v>
       </c>
@@ -4326,7 +4332,7 @@
         <v>-7.4833638394240509E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>41759</v>
       </c>
@@ -4349,7 +4355,7 @@
         <v>-3.74762275474253E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>41790</v>
       </c>
@@ -4372,7 +4378,7 @@
         <v>7.8577068039236142E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>41820</v>
       </c>
@@ -4395,7 +4401,7 @@
         <v>5.2720398330555973E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>41851</v>
       </c>
@@ -4418,7 +4424,7 @@
         <v>-6.0541136141038177E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>41882</v>
       </c>
@@ -4441,7 +4447,7 @@
         <v>4.8296287548055039E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>41912</v>
       </c>
@@ -4464,7 +4470,7 @@
         <v>-5.9282568263819058E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>41943</v>
       </c>
@@ -4487,7 +4493,7 @@
         <v>6.5935030275499296E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>41973</v>
       </c>
@@ -4510,7 +4516,7 @@
         <v>1.1148023671390119E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>42004</v>
       </c>
@@ -4533,7 +4539,7 @@
         <v>2.8930333265287711E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>42035</v>
       </c>
@@ -4556,7 +4562,7 @@
         <v>-3.2770299494886863E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>42063</v>
       </c>
@@ -4579,7 +4585,7 @@
         <v>5.9464046848752623E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>42094</v>
       </c>
@@ -4602,7 +4608,7 @@
         <v>1.7701664738250859E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>42124</v>
       </c>
@@ -4625,7 +4631,7 @@
         <v>-2.5649764275339489E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>42155</v>
       </c>
@@ -4648,7 +4654,7 @@
         <v>2.2363614155479491E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>42185</v>
       </c>
@@ -4671,7 +4677,7 @@
         <v>7.8291029024701864E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>42216</v>
       </c>
@@ -4694,7 +4700,7 @@
         <v>-1.103725004535239E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>42247</v>
       </c>
@@ -4717,7 +4723,7 @@
         <v>-6.3109555653225735E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>42277</v>
       </c>
@@ -4740,7 +4746,7 @@
         <v>-4.9362469286576172E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>42308</v>
       </c>
@@ -4763,7 +4769,7 @@
         <v>5.6227295019203982E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>42338</v>
       </c>
@@ -4786,7 +4792,7 @@
         <v>3.2599567153892117E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>42369</v>
       </c>
@@ -4809,7 +4815,7 @@
         <v>-5.030545804684472E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>42400</v>
       </c>
@@ -4832,7 +4838,7 @@
         <v>-8.5774781399222122E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>42429</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>-2.2341737056597029E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>42460</v>
       </c>
@@ -4878,7 +4884,7 @@
         <v>8.013122113350879E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>42490</v>
       </c>
@@ -4901,7 +4907,7 @@
         <v>1.6722347882382142E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>42521</v>
       </c>
@@ -4924,7 +4930,7 @@
         <v>2.240403115339484E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>42551</v>
       </c>
@@ -4947,7 +4953,7 @@
         <v>-1.739591762983661E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>42582</v>
       </c>
@@ -4970,7 +4976,7 @@
         <v>5.8744026923184027E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>42613</v>
       </c>
@@ -4993,7 +4999,7 @@
         <v>1.7840864932395339E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>42643</v>
       </c>
@@ -5016,7 +5022,7 @@
         <v>1.074078501124842E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>42674</v>
       </c>
@@ -5039,7 +5045,7 @@
         <v>-4.5970549689125839E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>42704</v>
       </c>
@@ -5062,7 +5068,7 @@
         <v>0.1106330584659105</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>42735</v>
       </c>
@@ -5085,7 +5091,7 @@
         <v>2.8843054436902719E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>42766</v>
       </c>
@@ -5108,7 +5114,7 @@
         <v>2.818098653692092E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>42794</v>
       </c>
@@ -5131,7 +5137,7 @@
         <v>1.9300708559139231E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>42825</v>
       </c>
@@ -5154,7 +5160,7 @@
         <v>2.5898548968461549E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>42855</v>
       </c>
@@ -5177,7 +5183,7 @@
         <v>1.149217781282807E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>42886</v>
       </c>
@@ -5200,7 +5206,7 @@
         <v>-1.9703160960030001E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>42916</v>
       </c>
@@ -5223,7 +5229,7 @@
         <v>3.3743781392489007E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>42947</v>
       </c>
@@ -5246,7 +5252,7 @@
         <v>8.5257622936827371E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>42978</v>
       </c>
@@ -5269,7 +5275,7 @@
         <v>-1.257904508633689E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>43008</v>
       </c>
@@ -5292,7 +5298,7 @@
         <v>6.3037898291989913E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>43039</v>
       </c>
@@ -5315,7 +5321,7 @@
         <v>7.2882393589737138E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>43069</v>
       </c>
@@ -5338,7 +5344,7 @@
         <v>2.9412169528728601E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>43100</v>
       </c>
@@ -5361,7 +5367,7 @@
         <v>-3.9830656375439144E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>43131</v>
       </c>
@@ -5384,7 +5390,7 @@
         <v>2.5580843264874979E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>43159</v>
       </c>
@@ -5407,7 +5413,7 @@
         <v>-3.8437214531656383E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>43190</v>
       </c>
@@ -5430,7 +5436,7 @@
         <v>1.2177525204761791E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>43220</v>
       </c>
@@ -5453,7 +5459,7 @@
         <v>9.8140879764150313E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>43251</v>
       </c>
@@ -5476,7 +5482,7 @@
         <v>6.1635462593664592E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>43281</v>
       </c>
@@ -5499,7 +5505,7 @@
         <v>6.1436944434722918E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>43312</v>
       </c>
@@ -5522,7 +5528,7 @@
         <v>1.649160752979606E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>43343</v>
       </c>
@@ -5545,7 +5551,7 @@
         <v>4.3105958242656277E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>43373</v>
       </c>
@@ -5568,7 +5574,7 @@
         <v>-2.3247768243955691E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>43404</v>
       </c>
@@ -5591,7 +5597,7 @@
         <v>-0.1098786279349008</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>43434</v>
       </c>
@@ -5614,7 +5620,7 @@
         <v>1.7263741160625571E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>43465</v>
       </c>
@@ -5637,7 +5643,7 @@
         <v>-0.11971972910599089</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>43496</v>
       </c>
@@ -5660,7 +5666,7 @@
         <v>0.11321893127052431</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>43524</v>
       </c>
@@ -5683,7 +5689,7 @@
         <v>5.1791434647304513E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>43555</v>
       </c>
@@ -5706,7 +5712,7 @@
         <v>-2.0932654588115881E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>43585</v>
       </c>
@@ -5729,7 +5735,7 @@
         <v>3.3966861801201453E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>43616</v>
       </c>
@@ -5752,7 +5758,7 @@
         <v>-7.8527093050940078E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>43646</v>
       </c>
@@ -5775,7 +5781,7 @@
         <v>6.9849109445870861E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>43677</v>
       </c>
@@ -5798,7 +5804,7 @@
         <v>6.8172525948215767E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>43708</v>
       </c>
@@ -5821,7 +5827,7 @@
         <v>-4.9310525632986657E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>43738</v>
       </c>
@@ -5844,7 +5850,7 @@
         <v>2.0369014705150509E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>43769</v>
       </c>
@@ -5867,7 +5873,7 @@
         <v>2.715775234754458E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>43799</v>
       </c>
@@ -5890,7 +5896,7 @@
         <v>4.065607966158491E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>43830</v>
       </c>
@@ -5913,7 +5919,7 @@
         <v>2.7866708458475161E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>43861</v>
       </c>
@@ -5936,7 +5942,7 @@
         <v>-3.102535573792831E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>43890</v>
       </c>
@@ -5959,7 +5965,7 @@
         <v>-8.8456880550268679E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>43921</v>
       </c>
@@ -5982,7 +5988,7 @@
         <v>-0.21477184475078559</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>43951</v>
       </c>
@@ -6005,7 +6011,7 @@
         <v>0.13847699347528411</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>43982</v>
       </c>
@@ -6028,7 +6034,7 @@
         <v>6.591959610979492E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>44012</v>
       </c>
@@ -6051,7 +6057,7 @@
         <v>3.4298265502350267E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>44043</v>
       </c>
@@ -6074,7 +6080,7 @@
         <v>2.919403432904422E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>44074</v>
       </c>
@@ -6097,7 +6103,7 @@
         <v>5.4763269436248103E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>44104</v>
       </c>
@@ -6120,7 +6126,7 @@
         <v>-3.2610314490387197E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>44135</v>
       </c>
@@ -6143,7 +6149,7 @@
         <v>2.2031313605544781E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>44165</v>
       </c>
@@ -6166,7 +6172,7 @@
         <v>0.1824412625647831</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>44196</v>
       </c>
@@ -6189,7 +6195,7 @@
         <v>8.6467233279219791E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>44227</v>
       </c>
@@ -6212,7 +6218,7 @@
         <v>4.845461776627058E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>44255</v>
       </c>
@@ -6235,7 +6241,7 @@
         <v>6.2025391701401089E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>44286</v>
       </c>
@@ -6258,7 +6264,7 @@
         <v>1.3950408456195881E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>44316</v>
       </c>
@@ -6281,7 +6287,7 @@
         <v>1.787806092088684E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>44347</v>
       </c>
@@ -6304,7 +6310,7 @@
         <v>2.712555519604587E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A120" s="2">
         <v>44377</v>
       </c>
@@ -6327,7 +6333,7 @@
         <v>1.8690843420986258E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A121" s="2">
         <v>44408</v>
       </c>
@@ -6350,7 +6356,7 @@
         <v>-3.6273311711919283E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A122" s="2">
         <v>44439</v>
       </c>
@@ -6373,7 +6379,7 @@
         <v>2.2031205427404329E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A123" s="2">
         <v>44469</v>
       </c>
@@ -6396,7 +6402,7 @@
         <v>-2.8803700585502749E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A124" s="2">
         <v>44500</v>
       </c>
@@ -6419,7 +6425,7 @@
         <v>4.2513991023543918E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A125" s="2">
         <v>44530</v>
       </c>
@@ -6442,7 +6448,7 @@
         <v>-4.3323583248623621E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A126" s="2">
         <v>44561</v>
       </c>
@@ -6465,7 +6471,7 @@
         <v>2.2712556163573479E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A127" s="2">
         <v>44592</v>
       </c>
@@ -6488,7 +6494,7 @@
         <v>-9.5347627515070088E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A128" s="2">
         <v>44620</v>
       </c>
@@ -6511,7 +6517,7 @@
         <v>1.0336105668164119E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A129" s="2">
         <v>44651</v>
       </c>
@@ -6534,7 +6540,7 @@
         <v>1.1573423556828329E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A130" s="2">
         <v>44681</v>
       </c>
@@ -6557,7 +6563,7 @@
         <v>-9.8991511137268229E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A131" s="2">
         <v>44712</v>
       </c>
@@ -6580,7 +6586,7 @@
         <v>1.9463007001370161E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A132" s="2">
         <v>44742</v>
       </c>
@@ -6603,7 +6609,7 @@
         <v>-8.3662611462856806E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A133" s="2">
         <v>44773</v>
       </c>
@@ -6626,7 +6632,7 @@
         <v>0.1056325587592826</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A134" s="2">
         <v>44804</v>
       </c>
@@ -6649,7 +6655,7 @@
         <v>-2.0026284361895241E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A135" s="2">
         <v>44834</v>
       </c>
@@ -6672,7 +6678,7 @@
         <v>-9.6601905550491862E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A136" s="2">
         <v>44865</v>
       </c>
@@ -6695,7 +6701,7 @@
         <v>0.1116296861160013</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A137" s="2">
         <v>44895</v>
       </c>
@@ -6718,7 +6724,7 @@
         <v>2.203698911670848E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A138" s="2">
         <v>44926</v>
       </c>
@@ -6741,7 +6747,7 @@
         <v>-6.5144163911122099E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A139" s="2">
         <v>44957</v>
       </c>
@@ -6764,7 +6770,7 @@
         <v>9.8187851699262252E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A140" s="2">
         <v>44985</v>
       </c>
@@ -6787,7 +6793,7 @@
         <v>-1.723425008172208E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A141" s="2">
         <v>45016</v>
       </c>
@@ -6810,7 +6816,7 @@
         <v>-4.8475586492693568E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A142" s="2">
         <v>45046</v>
       </c>
@@ -6833,7 +6839,7 @@
         <v>-1.793743498576339E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A143" s="2">
         <v>45077</v>
       </c>
@@ -6856,7 +6862,7 @@
         <v>-8.1615730392644581E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A144" s="2">
         <v>45107</v>
       </c>
@@ -6879,7 +6885,7 @@
         <v>8.0671494251540743E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A145" s="2">
         <v>45138</v>
       </c>
@@ -6902,7 +6908,7 @@
         <v>6.1087913697394747E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A146" s="2">
         <v>45169</v>
       </c>
@@ -6934,11 +6940,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
@@ -6955,7 +6961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>40786</v>
       </c>
@@ -6969,7 +6975,7 @@
         <v>-0.21086684055418181</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>40816</v>
       </c>
@@ -6983,7 +6989,7 @@
         <v>-0.20698832417582419</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>40847</v>
       </c>
@@ -6997,7 +7003,7 @@
         <v>0.32607989607015281</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>40877</v>
       </c>
@@ -7011,7 +7017,7 @@
         <v>-3.3553759490570823E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>40908</v>
       </c>
@@ -7025,7 +7031,7 @@
         <v>2.2976854198344391E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>40939</v>
       </c>
@@ -7039,7 +7045,7 @@
         <v>0.13897605284888501</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>40968</v>
       </c>
@@ -7053,7 +7059,7 @@
         <v>0.13238599289494671</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>40999</v>
       </c>
@@ -7067,7 +7073,7 @@
         <v>9.2931685767334571E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>41029</v>
       </c>
@@ -7081,7 +7087,7 @@
         <v>-2.3813010749538569E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>41060</v>
       </c>
@@ -7095,7 +7101,7 @@
         <v>-0.17348775804128669</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>41090</v>
       </c>
@@ -7109,7 +7115,7 @@
         <v>0.11468089740797199</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>41121</v>
       </c>
@@ -7123,7 +7129,7 @@
         <v>3.5173424523693209E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>41152</v>
       </c>
@@ -7137,7 +7143,7 @@
         <v>6.5250904514708052E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>41182</v>
       </c>
@@ -7151,7 +7157,7 @@
         <v>7.5194187660592382E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>41213</v>
       </c>
@@ -7165,7 +7171,7 @@
         <v>-5.9634665567916412E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>41243</v>
       </c>
@@ -7179,7 +7185,7 @@
         <v>1.010691125781382E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>41274</v>
       </c>
@@ -7193,7 +7199,7 @@
         <v>2.816657027183345E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>41305</v>
       </c>
@@ -7207,7 +7213,7 @@
         <v>0.15387860718906449</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>41333</v>
       </c>
@@ -7221,7 +7227,7 @@
         <v>3.5588056063375888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>41364</v>
       </c>
@@ -7235,7 +7241,7 @@
         <v>0.110391903024597</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>41394</v>
       </c>
@@ -7249,7 +7255,7 @@
         <v>5.4478007419183738E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>41425</v>
       </c>
@@ -7263,7 +7269,7 @@
         <v>6.80470399035078E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>41455</v>
       </c>
@@ -7277,7 +7283,7 @@
         <v>-5.2249200075286988E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>41486</v>
       </c>
@@ -7291,7 +7297,7 @@
         <v>0.16409818485125299</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>41517</v>
       </c>
@@ -7305,7 +7311,7 @@
         <v>-9.2140505314157961E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>41547</v>
       </c>
@@ -7319,7 +7325,7 @@
         <v>9.5986169573060609E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>41578</v>
       </c>
@@ -7333,7 +7339,7 @@
         <v>0.137610589122831</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>41608</v>
       </c>
@@ -7347,7 +7353,7 @@
         <v>8.8741522230595393E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>41639</v>
       </c>
@@ -7361,7 +7367,7 @@
         <v>7.5361997840471817E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>41670</v>
       </c>
@@ -7375,7 +7381,7 @@
         <v>-0.1071548106382431</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>41698</v>
       </c>
@@ -7389,7 +7395,7 @@
         <v>0.1365379624556646</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>41729</v>
       </c>
@@ -7406,7 +7412,7 @@
         <v>2.142639671182844E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>41759</v>
       </c>
@@ -7423,7 +7429,7 @@
         <v>1.6580349491411631E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>41790</v>
       </c>
@@ -7440,7 +7446,7 @@
         <v>6.6229291892684339E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>41820</v>
       </c>
@@ -7457,7 +7463,7 @@
         <v>6.2252930459592459E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>41851</v>
       </c>
@@ -7474,7 +7480,7 @@
         <v>-4.4409207602528422E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>41882</v>
       </c>
@@ -7491,7 +7497,7 @@
         <v>0.1195408007766201</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>41912</v>
       </c>
@@ -7508,7 +7514,7 @@
         <v>-4.4354147551396987E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>41943</v>
       </c>
@@ -7525,7 +7531,7 @@
         <v>6.0329183372019417E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>41973</v>
       </c>
@@ -7542,7 +7548,7 @@
         <v>8.3404644868554589E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>42004</v>
       </c>
@@ -7559,7 +7565,7 @@
         <v>-1.53563556208669E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>42035</v>
       </c>
@@ -7576,7 +7582,7 @@
         <v>-9.4722408775464673E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>42063</v>
       </c>
@@ -7593,7 +7599,7 @@
         <v>0.17485291541734951</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>42094</v>
       </c>
@@ -7610,7 +7616,7 @@
         <v>-5.2840216447558867E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>42124</v>
       </c>
@@ -7627,7 +7633,7 @@
         <v>2.5926406044556542E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>42155</v>
       </c>
@@ -7644,7 +7650,7 @@
         <v>3.4323724254950561E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>42185</v>
       </c>
@@ -7661,7 +7667,7 @@
         <v>-6.2084973080514187E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>42216</v>
       </c>
@@ -7678,7 +7684,7 @@
         <v>6.1747576428558222E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>42247</v>
       </c>
@@ -7695,7 +7701,7 @@
         <v>-0.18865609912112369</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>42277</v>
       </c>
@@ -7712,7 +7718,7 @@
         <v>-8.6356420031751813E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>42308</v>
       </c>
@@ -7729,7 +7735,7 @@
         <v>0.26788183978155261</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>42338</v>
       </c>
@@ -7746,7 +7752,7 @@
         <v>8.1578235858996706E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>42369</v>
       </c>
@@ -7763,7 +7769,7 @@
         <v>-6.0563744983076477E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>42400</v>
       </c>
@@ -7780,7 +7786,7 @@
         <v>-0.15378254663582219</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>42429</v>
       </c>
@@ -7797,7 +7803,7 @@
         <v>-1.6797924688528702E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>42460</v>
       </c>
@@ -7814,7 +7820,7 @@
         <v>0.21496941516108811</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>42490</v>
       </c>
@@ -7831,7 +7837,7 @@
         <v>8.0632595824243758E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>42521</v>
       </c>
@@ -7848,7 +7854,7 @@
         <v>4.6543529502685477E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>42551</v>
       </c>
@@ -7865,7 +7871,7 @@
         <v>-2.0492181586574398E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>42582</v>
       </c>
@@ -7882,7 +7888,7 @@
         <v>0.1113197424892705</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>42613</v>
       </c>
@@ -7899,7 +7905,7 @@
         <v>1.082007873687951E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>42643</v>
       </c>
@@ -7916,7 +7922,7 @@
         <v>-5.3459929994927879E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>42674</v>
       </c>
@@ -7933,7 +7939,7 @@
         <v>-5.6221475500275793E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>42704</v>
       </c>
@@ -7950,7 +7956,7 @@
         <v>0.1105058986077161</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>42735</v>
       </c>
@@ -7967,7 +7973,7 @@
         <v>5.9600430673525377E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>42766</v>
       </c>
@@ -7984,7 +7990,7 @@
         <v>5.1355582652155007E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>42794</v>
       </c>
@@ -8001,7 +8007,7 @@
         <v>0.1190999491698943</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>42825</v>
       </c>
@@ -8018,7 +8024,7 @@
         <v>-2.1814645879847379E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>42855</v>
       </c>
@@ -8035,7 +8041,7 @@
         <v>2.770297994563253E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>42886</v>
       </c>
@@ -8055,7 +8061,7 @@
         <v>3.6993830202686213E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>42916</v>
       </c>
@@ -8075,7 +8081,7 @@
         <v>1.514796031932253E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>42947</v>
       </c>
@@ -8095,7 +8101,7 @@
         <v>5.8727666004918737E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>42978</v>
       </c>
@@ -8115,7 +8121,7 @@
         <v>2.087822898883207E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>43008</v>
       </c>
@@ -8135,7 +8141,7 @@
         <v>5.6896127979980671E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>43039</v>
       </c>
@@ -8155,7 +8161,7 @@
         <v>6.8345894067035395E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>43069</v>
       </c>
@@ -8175,7 +8181,7 @@
         <v>8.8723002186538391E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>43100</v>
       </c>
@@ -8195,7 +8201,7 @@
         <v>3.4546371563197287E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>43131</v>
       </c>
@@ -8215,7 +8221,7 @@
         <v>0.1821647546599674</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>43159</v>
       </c>
@@ -8235,7 +8241,7 @@
         <v>-0.1353209986625056</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>43190</v>
       </c>
@@ -8255,7 +8261,7 @@
         <v>-8.6874884526310869E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>43220</v>
       </c>
@@ -8275,7 +8281,7 @@
         <v>-1.3787067448404191E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>43251</v>
       </c>
@@ -8295,7 +8301,7 @@
         <v>6.4648368476852403E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>43281</v>
       </c>
@@ -8315,7 +8321,7 @@
         <v>1.285268538803686E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>43312</v>
       </c>
@@ -8335,7 +8341,7 @@
         <v>0.1072934555099652</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>43343</v>
       </c>
@@ -8355,7 +8361,7 @@
         <v>9.0926311053934006E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>43373</v>
       </c>
@@ -8375,7 +8381,7 @@
         <v>1.196987454963749E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>43404</v>
       </c>
@@ -8395,7 +8401,7 @@
         <v>-0.20778686913098329</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>43434</v>
       </c>
@@ -8415,7 +8421,7 @@
         <v>4.2757102118903927E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>43465</v>
       </c>
@@ -8435,7 +8441,7 @@
         <v>-0.26220683686715712</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>43496</v>
       </c>
@@ -8455,7 +8461,7 @@
         <v>0.23893281096044669</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>43524</v>
       </c>
@@ -8475,7 +8481,7 @@
         <v>9.2831478439522108E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>43555</v>
       </c>
@@ -8495,7 +8501,7 @@
         <v>4.8494063321680818E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>43585</v>
       </c>
@@ -8515,7 +8521,7 @@
         <v>0.1181005420412482</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>43616</v>
       </c>
@@ -8535,7 +8541,7 @@
         <v>-0.18892674239009161</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>43646</v>
       </c>
@@ -8555,7 +8561,7 @@
         <v>0.21365897660179309</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>43677</v>
       </c>
@@ -8575,7 +8581,7 @@
         <v>3.8040112160899087E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>43708</v>
       </c>
@@ -8595,7 +8601,7 @@
         <v>-6.6179209292065888E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>43738</v>
       </c>
@@ -8615,7 +8621,7 @@
         <v>5.2963180966247858E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>43769</v>
       </c>
@@ -8635,7 +8641,7 @@
         <v>5.6992493922688459E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>43799</v>
       </c>
@@ -8655,7 +8661,7 @@
         <v>0.107327511220904</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>43830</v>
       </c>
@@ -8675,7 +8681,7 @@
         <v>8.3806483439484269E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>43861</v>
       </c>
@@ -8695,7 +8701,7 @@
         <v>-9.1439107758407578E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>43890</v>
       </c>
@@ -8715,7 +8721,7 @@
         <v>-0.23035915441445401</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>43921</v>
       </c>
@@ -8735,7 +8741,7 @@
         <v>-0.48125408676875348</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>43951</v>
       </c>
@@ -8755,7 +8761,7 @@
         <v>0.37169574871933908</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>43982</v>
       </c>
@@ -8775,7 +8781,7 @@
         <v>0.13377000833458011</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>44012</v>
       </c>
@@ -8795,7 +8801,7 @@
         <v>3.2350030630036157E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>44043</v>
       </c>
@@ -8815,7 +8821,7 @@
         <v>0.17696222754764371</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>44074</v>
       </c>
@@ -8835,7 +8841,7 @@
         <v>0.22045585879779539</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>44104</v>
       </c>
@@ -8855,7 +8861,7 @@
         <v>-0.1225666219660233</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="2">
         <v>44135</v>
       </c>
@@ -8875,7 +8881,7 @@
         <v>-8.4779585391646872E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="2">
         <v>44165</v>
       </c>
@@ -8895,7 +8901,7 @@
         <v>0.3519609666530803</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="2">
         <v>44196</v>
       </c>
@@ -8915,7 +8921,7 @@
         <v>0.1114210449290209</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="2">
         <v>44227</v>
       </c>
@@ -8935,7 +8941,7 @@
         <v>-3.7080246604708322E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="2">
         <v>44255</v>
       </c>
@@ -8955,7 +8961,7 @@
         <v>7.7421048745066834E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="2">
         <v>44286</v>
       </c>
@@ -8975,7 +8981,7 @@
         <v>0.13330541065377141</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="2">
         <v>44316</v>
       </c>
@@ -8995,7 +9001,7 @@
         <v>0.1617210948349235</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="2">
         <v>44347</v>
       </c>
@@ -9015,7 +9021,7 @@
         <v>1.3627371968642389E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="2">
         <v>44377</v>
       </c>
@@ -9035,7 +9041,7 @@
         <v>6.5895041180834335E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="2">
         <v>44408</v>
       </c>
@@ -9055,7 +9061,7 @@
         <v>6.9318114898469396E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="2">
         <v>44439</v>
       </c>
@@ -9075,7 +9081,7 @@
         <v>8.9732100391010094E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="2">
         <v>44469</v>
       </c>
@@ -9095,7 +9101,7 @@
         <v>-0.13940880815208889</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="2">
         <v>44500</v>
       </c>
@@ -9115,7 +9121,7 @@
         <v>0.2189787776223677</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" s="2">
         <v>44530</v>
       </c>
@@ -9135,7 +9141,7 @@
         <v>-2.7126611290346329E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" s="2">
         <v>44561</v>
       </c>
@@ -9155,7 +9161,7 @@
         <v>0.13180118482416711</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" s="2">
         <v>44592</v>
       </c>
@@ -9175,7 +9181,7 @@
         <v>-0.15888866497671911</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" s="2">
         <v>44620</v>
       </c>
@@ -9195,7 +9201,7 @@
         <v>-9.8504145518741537E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" s="2">
         <v>44651</v>
       </c>
@@ -9215,7 +9221,7 @@
         <v>0.1007243931480766</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" s="2">
         <v>44681</v>
       </c>
@@ -9235,7 +9241,7 @@
         <v>-0.25412606785336461</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" s="2">
         <v>44712</v>
       </c>
@@ -9255,7 +9261,7 @@
         <v>-2.1279812928466039E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" s="2">
         <v>44742</v>
       </c>
@@ -9275,7 +9281,7 @@
         <v>-0.2493009633106377</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" s="2">
         <v>44773</v>
       </c>
@@ -9295,7 +9301,7 @@
         <v>0.28620663667563312</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" s="2">
         <v>44804</v>
       </c>
@@ -9315,7 +9321,7 @@
         <v>-0.13333303285098411</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" s="2">
         <v>44834</v>
       </c>
@@ -9335,7 +9341,7 @@
         <v>-0.26910265311376169</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" s="2">
         <v>44865</v>
       </c>
@@ -9355,7 +9361,7 @@
         <v>0.2305543992969947</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" s="2">
         <v>44895</v>
       </c>
@@ -9375,7 +9381,7 @@
         <v>0.1438781322007732</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" s="2">
         <v>44926</v>
       </c>
@@ -9395,7 +9401,7 @@
         <v>-0.17726110077644769</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" s="2">
         <v>44957</v>
       </c>
@@ -9415,7 +9421,7 @@
         <v>0.1812604641875184</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" s="2">
         <v>44985</v>
       </c>
@@ -9435,7 +9441,7 @@
         <v>-8.7314508033433991E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" s="2">
         <v>45016</v>
       </c>
@@ -9455,7 +9461,7 @@
         <v>9.421731102398101E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" s="2">
         <v>45046</v>
       </c>
@@ -9475,7 +9481,7 @@
         <v>3.6038217854268861E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" s="2">
         <v>45077</v>
       </c>
@@ -9495,7 +9501,7 @@
         <v>-1.500573083187517E-3</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" s="2">
         <v>45107</v>
       </c>
@@ -9515,7 +9521,7 @@
         <v>0.19124684393494309</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" s="2">
         <v>45138</v>
       </c>
@@ -9535,7 +9541,7 @@
         <v>8.9488276165198721E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" s="2">
         <v>45169</v>
       </c>

</xml_diff>